<commit_message>
Improved data saving and added comments
</commit_message>
<xml_diff>
--- a/PE_test.Server/devices.xlsx
+++ b/PE_test.Server/devices.xlsx
@@ -19,49 +19,49 @@
     <x:t>AŠG</x:t>
   </x:si>
   <x:si>
+    <x:t>NŠG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AB Panevėžio energija konkurenciniai įrenginiai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AB Panevėžio energija piko/rezervo įrenginiai</x:t>
+  </x:si>
+  <x:si>
     <x:t>AB Panevėžio stiklas</x:t>
   </x:si>
   <x:si>
+    <x:t>UAB Biokuro energija</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRK-1 GK Nr.6 ir Nr.7 kogeneracinis blokas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRK-1 VŠK Nr.8 ir Nr.9 blokas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PEI katilinė VŠK Nr.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRK-1 VŠK Nr.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mw</x:t>
+  </x:si>
+  <x:si>
     <x:t>Šilumos gamyba</x:t>
   </x:si>
   <x:si>
+    <x:t>T1 (C)</x:t>
+  </x:si>
+  <x:si>
     <x:t>Termofikacinio vandens</x:t>
   </x:si>
   <x:si>
-    <x:t>Mw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T1 (C)</x:t>
-  </x:si>
-  <x:si>
     <x:t>P1 (bar)</x:t>
   </x:si>
   <x:si>
     <x:t>P2 (bar)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NŠG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UAB Biokuro energija</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AB Panevėžio energija konkurenciniai įrenginiai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRK-1 GK Nr.6 ir Nr.7 kogeneracinis blokas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRK-1 VŠK Nr.8 ir Nr.9 blokas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PEI katilinė VŠK Nr.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRK-1 VŠK Nr.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AB Panevėžio energija piko/rezervo įrenginiai</x:t>
   </x:si>
   <x:si>
     <x:t>-</x:t>
@@ -71,11 +71,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
+  <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="164" formatCode="0.0"/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -91,7 +100,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -103,6 +112,23 @@
         <x:color rgb="FF000000"/>
       </x:top>
       <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="hair">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="hair">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="hair">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="hair">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -110,14 +136,28 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -420,254 +460,330 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="2" max="4" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="6" max="8" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="10" max="12" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="14" max="16" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="18" max="20" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="21" max="21" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="22" max="24" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="25" max="25" width="15.567768" style="0" customWidth="1"/>
+    <x:col min="26" max="28" width="9.710625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:28">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="Y1" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
+      <x:c r="B1" s="1"/>
+      <x:c r="C1" s="1"/>
+      <x:c r="D1" s="1"/>
+      <x:c r="E1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F1" s="1"/>
+      <x:c r="G1" s="1"/>
+      <x:c r="H1" s="1"/>
+      <x:c r="I1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="J1" s="1"/>
+      <x:c r="K1" s="1"/>
+      <x:c r="L1" s="1"/>
+      <x:c r="M1" s="1"/>
+      <x:c r="N1" s="1"/>
+      <x:c r="O1" s="1"/>
+      <x:c r="P1" s="1"/>
+      <x:c r="Q1" s="1"/>
+      <x:c r="R1" s="1"/>
+      <x:c r="S1" s="1"/>
+      <x:c r="T1" s="1"/>
+      <x:c r="U1" s="1"/>
+      <x:c r="V1" s="1"/>
+      <x:c r="W1" s="1"/>
+      <x:c r="X1" s="1"/>
+      <x:c r="Y1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="Z1" s="1"/>
+      <x:c r="AA1" s="1"/>
+      <x:c r="AB1" s="1"/>
     </x:row>
     <x:row r="2" spans="1:28">
-      <x:c r="A2" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="A2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="1"/>
+      <x:c r="C2" s="1"/>
+      <x:c r="D2" s="1"/>
+      <x:c r="E2" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F2" s="1"/>
+      <x:c r="G2" s="1"/>
+      <x:c r="H2" s="1"/>
+      <x:c r="I2" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="J2" s="1"/>
+      <x:c r="K2" s="1"/>
+      <x:c r="L2" s="1"/>
+      <x:c r="M2" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="N2" s="1"/>
+      <x:c r="O2" s="1"/>
+      <x:c r="P2" s="1"/>
+      <x:c r="Q2" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="R2" s="1"/>
+      <x:c r="S2" s="1"/>
+      <x:c r="T2" s="1"/>
+      <x:c r="U2" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="U2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
+      <x:c r="V2" s="1"/>
+      <x:c r="W2" s="1"/>
+      <x:c r="X2" s="1"/>
+      <x:c r="Y2" s="1"/>
+      <x:c r="Z2" s="1"/>
+      <x:c r="AA2" s="1"/>
+      <x:c r="AB2" s="1"/>
     </x:row>
     <x:row r="3" spans="1:28">
-      <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="M3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="N3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="Q3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="R3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="U3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="V3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="Y3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="Z3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
+      <x:c r="A3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="2"/>
+      <x:c r="D3" s="2"/>
+      <x:c r="E3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G3" s="2"/>
+      <x:c r="H3" s="2"/>
+      <x:c r="I3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="K3" s="2"/>
+      <x:c r="L3" s="2"/>
+      <x:c r="M3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="N3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O3" s="2"/>
+      <x:c r="P3" s="2"/>
+      <x:c r="Q3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="R3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="S3" s="2"/>
+      <x:c r="T3" s="2"/>
+      <x:c r="U3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="V3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="W3" s="2"/>
+      <x:c r="X3" s="2"/>
+      <x:c r="Y3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="Z3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="AA3" s="2"/>
+      <x:c r="AB3" s="2"/>
     </x:row>
     <x:row r="4" spans="1:28">
-      <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="K4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="L4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="M4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="O4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="P4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="Q4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="R4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="S4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="T4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="U4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="V4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="W4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="X4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="Y4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="Z4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="AA4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="AB4" s="0" t="s">
-        <x:v>7</x:v>
+      <x:c r="A4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="L4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="M4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="N4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="O4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Q4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="R4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="S4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="T4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="U4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="V4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="W4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="X4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Y4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="Z4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="AA4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="AB4" s="2" t="s">
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:28">
-      <x:c r="A5" s="0">
+      <x:c r="A5" s="2">
         <x:v>0.4</x:v>
       </x:c>
-      <x:c r="B5" s="0">
+      <x:c r="B5" s="2">
         <x:v>65.9</x:v>
       </x:c>
-      <x:c r="C5" s="0">
+      <x:c r="C5" s="2">
         <x:v>7.80000019073486</x:v>
       </x:c>
-      <x:c r="D5" s="0">
+      <x:c r="D5" s="2">
         <x:v>1.20000004768372</x:v>
       </x:c>
-      <x:c r="E5" s="0">
+      <x:c r="E5" s="2">
         <x:v>9.5</x:v>
       </x:c>
-      <x:c r="F5" s="0">
+      <x:c r="F5" s="2">
         <x:v>64.7</x:v>
       </x:c>
-      <x:c r="G5" s="0">
+      <x:c r="G5" s="2">
         <x:v>6.69999980926514</x:v>
       </x:c>
-      <x:c r="H5" s="0">
+      <x:c r="H5" s="2">
         <x:v>1.29999995231628</x:v>
       </x:c>
-      <x:c r="I5" s="0">
+      <x:c r="I5" s="2">
         <x:v>16.7</x:v>
       </x:c>
-      <x:c r="J5" s="0">
+      <x:c r="J5" s="2">
         <x:v>64.7</x:v>
       </x:c>
-      <x:c r="K5" s="0">
+      <x:c r="K5" s="2">
         <x:v>6.69999980926514</x:v>
       </x:c>
-      <x:c r="L5" s="0">
+      <x:c r="L5" s="2">
         <x:v>1.29999995231628</x:v>
       </x:c>
-      <x:c r="M5" s="0">
+      <x:c r="M5" s="2">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="N5" s="0">
+      <x:c r="N5" s="2">
         <x:v>65.1</x:v>
       </x:c>
-      <x:c r="O5" s="0">
+      <x:c r="O5" s="2">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="P5" s="0">
+      <x:c r="P5" s="2">
         <x:v>2.09999990463257</x:v>
       </x:c>
-      <x:c r="Q5" s="0">
+      <x:c r="Q5" s="2">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="R5" s="0">
+      <x:c r="R5" s="2">
         <x:v>65.1</x:v>
       </x:c>
-      <x:c r="S5" s="0">
+      <x:c r="S5" s="2">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="T5" s="0">
+      <x:c r="T5" s="2">
         <x:v>2.09999990463257</x:v>
       </x:c>
-      <x:c r="U5" s="0" t="s">
+      <x:c r="U5" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="V5" s="0" t="s">
+      <x:c r="V5" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="W5" s="0">
+      <x:c r="W5" s="2">
         <x:v>7.40000009536743</x:v>
       </x:c>
-      <x:c r="X5" s="0">
+      <x:c r="X5" s="2">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="Y5" s="0">
+      <x:c r="Y5" s="2">
         <x:v>4.4</x:v>
       </x:c>
-      <x:c r="Z5" s="0" t="s">
+      <x:c r="Z5" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="AA5" s="0">
+      <x:c r="AA5" s="2">
         <x:v>7.40000009536743</x:v>
       </x:c>
-      <x:c r="AB5" s="0">
+      <x:c r="AB5" s="2">
         <x:v>2</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Improved temp and pressures functions
</commit_message>
<xml_diff>
--- a/PE_test.Server/devices.xlsx
+++ b/PE_test.Server/devices.xlsx
@@ -706,61 +706,61 @@
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="B5" s="2">
-        <x:v>65.9</x:v>
+        <x:v>65.93</x:v>
       </x:c>
       <x:c r="C5" s="2">
-        <x:v>7.80000019073486</x:v>
+        <x:v>7.76262235641479</x:v>
       </x:c>
       <x:c r="D5" s="2">
-        <x:v>1.20000004768372</x:v>
+        <x:v>1.19393062591553</x:v>
       </x:c>
       <x:c r="E5" s="2">
         <x:v>9.5</x:v>
       </x:c>
       <x:c r="F5" s="2">
-        <x:v>64.7</x:v>
+        <x:v>64.66</x:v>
       </x:c>
       <x:c r="G5" s="2">
-        <x:v>6.69999980926514</x:v>
+        <x:v>6.74870824813843</x:v>
       </x:c>
       <x:c r="H5" s="2">
-        <x:v>1.29999995231628</x:v>
+        <x:v>1.30078768730164</x:v>
       </x:c>
       <x:c r="I5" s="2">
         <x:v>16.7</x:v>
       </x:c>
       <x:c r="J5" s="2">
-        <x:v>64.7</x:v>
+        <x:v>64.66</x:v>
       </x:c>
       <x:c r="K5" s="2">
-        <x:v>6.69999980926514</x:v>
+        <x:v>6.74870824813843</x:v>
       </x:c>
       <x:c r="L5" s="2">
-        <x:v>1.29999995231628</x:v>
+        <x:v>1.30078768730164</x:v>
       </x:c>
       <x:c r="M5" s="2">
         <x:v>0</x:v>
       </x:c>
       <x:c r="N5" s="2">
-        <x:v>65.1</x:v>
+        <x:v>65.06</x:v>
       </x:c>
       <x:c r="O5" s="2">
-        <x:v>8</x:v>
+        <x:v>7.98389196395874</x:v>
       </x:c>
       <x:c r="P5" s="2">
-        <x:v>2.09999990463257</x:v>
+        <x:v>2.12885189056396</x:v>
       </x:c>
       <x:c r="Q5" s="2">
         <x:v>0</x:v>
       </x:c>
       <x:c r="R5" s="2">
-        <x:v>65.1</x:v>
+        <x:v>65.06</x:v>
       </x:c>
       <x:c r="S5" s="2">
-        <x:v>8</x:v>
+        <x:v>7.98389196395874</x:v>
       </x:c>
       <x:c r="T5" s="2">
-        <x:v>2.09999990463257</x:v>
+        <x:v>2.12885189056396</x:v>
       </x:c>
       <x:c r="U5" s="2" t="s">
         <x:v>16</x:v>
@@ -769,10 +769,10 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="W5" s="2">
-        <x:v>7.40000009536743</x:v>
+        <x:v>7.42410612106323</x:v>
       </x:c>
       <x:c r="X5" s="2">
-        <x:v>2</x:v>
+        <x:v>2.03520464897156</x:v>
       </x:c>
       <x:c r="Y5" s="2">
         <x:v>4.4</x:v>
@@ -781,10 +781,10 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="AA5" s="2">
-        <x:v>7.40000009536743</x:v>
+        <x:v>7.42410612106323</x:v>
       </x:c>
       <x:c r="AB5" s="2">
-        <x:v>2</x:v>
+        <x:v>2.03520464897156</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>